<commit_message>
Updated BOM, and CAD pictures
</commit_message>
<xml_diff>
--- a/Records/KBC_Main_PCB/Kettlebell_counter_BOM.xlsx
+++ b/Records/KBC_Main_PCB/Kettlebell_counter_BOM.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eh-b\Dropbox\KiCad_projects\Remote_for_KBC\KBC_main_PCB\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eh-b\Dropbox\VultureWoodElectric\GitHub\KettlebellCounter\Records\KBC_Main_PCB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C8A6F34B-642B-4F4C-8827-269F9E2E5A01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A204A17-977E-4C66-8844-B0C8A26730AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="130">
   <si>
     <t>Reference Name</t>
   </si>
@@ -99,15 +99,9 @@
     <t>Buzzer</t>
   </si>
   <si>
-    <t>https://www.aliexpress.com/item/1005002502965743.html?spm=a2g0o.productlist.0.0.59673354vAWSJq&amp;algo_pvid=fd497dc6-8f06-4228-a8ab-6e754e1d8385&amp;algo_exp_id=fd497dc6-8f06-4228-a8ab-6e754e1d8385-0&amp;pdp_ext_f=%7B%22sku_id%22%3A%2212000020907161432%22%7D&amp;pdp_npi=2%40dis%21EUR%211.4%211.2%21%21%21%21%21%402101d8f416696619758945568ee2b1%2112000020907161432%21sea&amp;curPageLogUid=dwk3DQFlSmcR</t>
-  </si>
-  <si>
     <t>5 V Square</t>
   </si>
   <si>
-    <t>Lantian Loud Buzzer</t>
-  </si>
-  <si>
     <t>Q1</t>
   </si>
   <si>
@@ -315,9 +309,6 @@
     <t>5V/2.5A</t>
   </si>
   <si>
-    <t>2.5 A is enough, maximum current is ~2.1A, Choose a semi long wire &gt;1m</t>
-  </si>
-  <si>
     <t>Cable</t>
   </si>
   <si>
@@ -373,6 +364,57 @@
   </si>
   <si>
     <t>Assorted wires for soldering swithces</t>
+  </si>
+  <si>
+    <t>https://www.aliexpress.com/item/1005001794416354.html?spm=a2g0o.productlist.main.1.147832f0BHWSHf&amp;algo_pvid=9bd9126c-7d79-4e7a-968f-7ad8407e91ee&amp;algo_exp_id=9bd9126c-7d79-4e7a-968f-7ad8407e91ee-0&amp;pdp_ext_f=%7B%22sku_id%22%3A%2212000017596091313%22%7D&amp;pdp_npi=2%40dis%21EUR%210.73%210.62%21%21%21%21%21%40210212c016734624397665408d0669%2112000017596091313%21sea&amp;curPageLogUid=xTvxAzRKwdO4</t>
+  </si>
+  <si>
+    <t>https://www.aliexpress.com/item/32988745109.html?spm=a2g0o.productlist.main.1.179d3106JMESZx&amp;algo_pvid=c6c8ff40-0080-43aa-b6a5-a599cb019953&amp;algo_exp_id=c6c8ff40-0080-43aa-b6a5-a599cb019953-0&amp;pdp_ext_f=%7B%22sku_id%22%3A%2266818227931%22%7D&amp;pdp_npi=2%40dis%21EUR%210.44%210.41%21%21%21%21%21%40211bf2da16734624632941647d06c0%2166818227931%21sea&amp;curPageLogUid=KB38y2zJRgmU</t>
+  </si>
+  <si>
+    <t>https://www.aliexpress.com/item/32783807336.html?spm=a2g0o.productlist.main.1.1acbbd8b8y6qKr&amp;algo_pvid=76c5bace-a9a9-48c2-8cb2-9cd607c66271&amp;algo_exp_id=76c5bace-a9a9-48c2-8cb2-9cd607c66271-0&amp;pdp_ext_f=%7B%22sku_id%22%3A%2263092260414%22%7D&amp;pdp_npi=2%40dis%21EUR%211.18%211.18%21%21%21%21%21%40212279b716734625064347781d06b7%2163092260414%21sea&amp;curPageLogUid=82CnQUzgYGWW</t>
+  </si>
+  <si>
+    <t>Round Piezoelectric buzzer</t>
+  </si>
+  <si>
+    <t>NUT</t>
+  </si>
+  <si>
+    <t>Hex nut 1/4" for mid frame, so tripod can be fixed</t>
+  </si>
+  <si>
+    <t>https://www.aliexpress.com/item/1005003345732578.html?spm=a2g0o.productlist.main.5.4f77123e12HYr5&amp;algo_pvid=e20bfe56-f369-412c-85a1-079ee66df5ba&amp;algo_exp_id=e20bfe56-f369-412c-85a1-079ee66df5ba-2&amp;pdp_ext_f=%7B%22sku_id%22%3A%2212000025331457469%22%7D&amp;pdp_npi=2%40dis%21EUR%212.73%212.4%21%21%21%21%21%40210218bf16734626637121900d06b0%2112000025331457469%21sea&amp;curPageLogUid=IAchS2ZKnS4B</t>
+  </si>
+  <si>
+    <t>Tripod</t>
+  </si>
+  <si>
+    <t>1/4-20 UNC</t>
+  </si>
+  <si>
+    <t>https://www.aliexpress.com/item/1005003504983409.html?spm=a2g0o.productlist.main.53.793371c5HVag0z&amp;algo_pvid=e7fdf71e-16fb-4298-b68a-4eb158ae8aa0&amp;algo_exp_id=e7fdf71e-16fb-4298-b68a-4eb158ae8aa0-26&amp;pdp_ext_f=%7B%22sku_id%22%3A%2212000028281940788%22%7D&amp;pdp_npi=2%40dis%21EUR%2115.73%2112.11%21%21%21%21%21%40211bf49716734626816148134d06eb%2112000028281940788%21sea&amp;curPageLogUid=XN0bGadiK4bz</t>
+  </si>
+  <si>
+    <t>with 1/4-20 unc thread</t>
+  </si>
+  <si>
+    <t>Tripod to mount the counter on</t>
+  </si>
+  <si>
+    <t>Bolt</t>
+  </si>
+  <si>
+    <t>A bolt UNC 1/4-20, for driving the nut into it´s place in the mid frame</t>
+  </si>
+  <si>
+    <t>https://www.aliexpress.com/item/33058333264.html?spm=a2g0o.productlist.main.1.5aba1f4csOX3Fc&amp;algo_pvid=a0e9c634-4914-4577-95dd-14a562b6f0bc&amp;algo_exp_id=a0e9c634-4914-4577-95dd-14a562b6f0bc-0&amp;pdp_ext_f=%7B%22sku_id%22%3A%2212000021338831054%22%7D&amp;pdp_npi=2%40dis%21EUR%214.77%213.29%21%21%21%21%21%4021021a7216734628444573764d06c1%2112000021338831054%21sea&amp;curPageLogUid=6rzwCtLGh5pI</t>
+  </si>
+  <si>
+    <t>5V power supply.  2.5A current, and 5.5-2.5mm plug</t>
+  </si>
+  <si>
+    <t>2.5 A should be enough, normal current is ~2.1A, Choose a semi long wire &gt;1m</t>
   </si>
 </sst>
 </file>
@@ -429,7 +471,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -441,6 +483,8 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -721,16 +765,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:F51"/>
+  <dimension ref="B2:F57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F51" sqref="F51"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="18.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.21875" customWidth="1"/>
     <col min="4" max="4" width="12.88671875" style="3" customWidth="1"/>
     <col min="5" max="5" width="59.5546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="84.6640625" bestFit="1" customWidth="1"/>
@@ -755,7 +799,7 @@
     </row>
     <row r="4" spans="2:6" ht="18" x14ac:dyDescent="0.35">
       <c r="B4" s="4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.3">
@@ -763,16 +807,16 @@
         <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D5" s="3">
         <v>2</v>
       </c>
       <c r="E5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F5" t="s">
-        <v>31</v>
+        <v>114</v>
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.3">
@@ -780,16 +824,16 @@
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D6" s="3">
         <v>3</v>
       </c>
       <c r="E6" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F6" t="s">
-        <v>36</v>
+        <v>113</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.3">
@@ -803,10 +847,10 @@
         <v>2</v>
       </c>
       <c r="E7" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F7" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.3">
@@ -828,135 +872,135 @@
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C9" t="s">
+        <v>36</v>
+      </c>
+      <c r="D9" s="3">
+        <v>1</v>
+      </c>
+      <c r="E9" t="s">
+        <v>39</v>
+      </c>
+      <c r="F9" t="s">
         <v>38</v>
-      </c>
-      <c r="D9" s="3">
-        <v>1</v>
-      </c>
-      <c r="E9" t="s">
-        <v>41</v>
-      </c>
-      <c r="F9" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C10" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D10" s="3">
         <v>2</v>
       </c>
       <c r="E10" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F10" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
+        <v>42</v>
+      </c>
+      <c r="C11" t="s">
+        <v>43</v>
+      </c>
+      <c r="D11" s="3">
+        <v>1</v>
+      </c>
+      <c r="E11" t="s">
         <v>44</v>
       </c>
-      <c r="C11" t="s">
+      <c r="F11" t="s">
         <v>45</v>
-      </c>
-      <c r="D11" s="3">
-        <v>1</v>
-      </c>
-      <c r="E11" t="s">
-        <v>46</v>
-      </c>
-      <c r="F11" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
+        <v>47</v>
+      </c>
+      <c r="C12" t="s">
+        <v>73</v>
+      </c>
+      <c r="D12" s="3">
+        <v>1</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="F12" t="s">
         <v>49</v>
-      </c>
-      <c r="C12" t="s">
-        <v>75</v>
-      </c>
-      <c r="D12" s="3">
-        <v>1</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="F12" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="13" spans="2:6" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C13" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D13" s="3">
         <v>1</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F13" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" t="s">
+        <v>26</v>
+      </c>
+      <c r="D14" s="3">
+        <v>1</v>
+      </c>
+      <c r="E14" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C14" t="s">
+      <c r="F14" t="s">
         <v>28</v>
-      </c>
-      <c r="D14" s="3">
-        <v>1</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="F14" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C15" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D15" s="3">
         <v>6</v>
       </c>
       <c r="E15" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F15" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C16" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D16" s="3">
         <v>1</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.3">
@@ -983,428 +1027,488 @@
       <c r="C18" t="s">
         <v>22</v>
       </c>
+      <c r="D18" s="3">
+        <v>1</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="F18" t="s">
+        <v>127</v>
+      </c>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B19" t="s">
-        <v>23</v>
-      </c>
-      <c r="C19" t="s">
-        <v>25</v>
-      </c>
-      <c r="D19" s="3">
-        <v>1</v>
-      </c>
       <c r="E19" t="s">
-        <v>26</v>
-      </c>
-      <c r="F19" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="20" spans="2:6" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="B20" t="s">
-        <v>18</v>
-      </c>
-      <c r="C20" t="s">
-        <v>16</v>
-      </c>
-      <c r="D20" s="3">
-        <v>2</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F20" t="s">
-        <v>14</v>
+        <v>92</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="E20" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
-        <v>56</v>
+        <v>23</v>
       </c>
       <c r="C21" t="s">
-        <v>57</v>
+        <v>24</v>
       </c>
       <c r="D21" s="3">
         <v>1</v>
       </c>
       <c r="E21" t="s">
-        <v>59</v>
+        <v>116</v>
       </c>
       <c r="F21" t="s">
-        <v>58</v>
+        <v>115</v>
       </c>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="E22" t="s">
-        <v>60</v>
+      <c r="B22" t="s">
+        <v>18</v>
+      </c>
+      <c r="C22" t="s">
+        <v>16</v>
+      </c>
+      <c r="D22" s="3">
+        <v>2</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>17</v>
       </c>
       <c r="F22" t="s">
-        <v>61</v>
+        <v>14</v>
       </c>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="C23" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="D23" s="3">
         <v>1</v>
       </c>
       <c r="E23" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="F23" t="s">
-        <v>70</v>
+        <v>56</v>
       </c>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B24" t="s">
-        <v>71</v>
-      </c>
-      <c r="C24" t="s">
-        <v>72</v>
-      </c>
-      <c r="D24" s="3">
-        <v>1</v>
-      </c>
       <c r="E24" t="s">
-        <v>74</v>
+        <v>58</v>
       </c>
       <c r="F24" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
-        <v>114</v>
+        <v>65</v>
+      </c>
+      <c r="C25" t="s">
+        <v>66</v>
+      </c>
+      <c r="D25" s="3">
+        <v>1</v>
       </c>
       <c r="E25" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="27" spans="2:6" ht="18" x14ac:dyDescent="0.35">
-      <c r="B27" s="4" t="s">
-        <v>64</v>
+        <v>67</v>
+      </c>
+      <c r="F25" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B26" t="s">
+        <v>69</v>
+      </c>
+      <c r="C26" t="s">
+        <v>70</v>
+      </c>
+      <c r="D26" s="3">
+        <v>1</v>
+      </c>
+      <c r="E26" t="s">
+        <v>72</v>
+      </c>
+      <c r="F26" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="27" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B27" t="s">
+        <v>111</v>
+      </c>
+      <c r="E27" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="28" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
-        <v>49</v>
-      </c>
-      <c r="C28" t="s">
-        <v>75</v>
+        <v>117</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>121</v>
       </c>
       <c r="D28" s="3">
         <v>1</v>
       </c>
-      <c r="E28" s="2" t="s">
-        <v>50</v>
+      <c r="E28" t="s">
+        <v>118</v>
       </c>
       <c r="F28" t="s">
-        <v>51</v>
+        <v>119</v>
       </c>
     </row>
     <row r="29" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
-        <v>76</v>
-      </c>
-      <c r="C29" t="s">
-        <v>78</v>
+        <v>125</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>121</v>
       </c>
       <c r="D29" s="3">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E29" t="s">
-        <v>35</v>
+        <v>126</v>
       </c>
       <c r="F29" t="s">
-        <v>36</v>
+        <v>122</v>
       </c>
     </row>
     <row r="30" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
-        <v>77</v>
-      </c>
-      <c r="C30" t="s">
-        <v>79</v>
+        <v>120</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>123</v>
       </c>
       <c r="D30" s="3">
         <v>1</v>
       </c>
       <c r="E30" t="s">
-        <v>81</v>
+        <v>124</v>
       </c>
       <c r="F30" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B31" t="s">
-        <v>89</v>
-      </c>
-      <c r="C31" t="s">
-        <v>86</v>
-      </c>
-      <c r="D31" s="3">
-        <v>4</v>
-      </c>
-      <c r="E31" t="s">
-        <v>87</v>
-      </c>
-      <c r="F31" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B32" t="s">
-        <v>65</v>
-      </c>
-      <c r="C32" t="s">
-        <v>82</v>
-      </c>
-      <c r="D32" s="3">
-        <v>1</v>
-      </c>
-      <c r="E32" t="s">
-        <v>84</v>
-      </c>
-      <c r="F32" t="s">
-        <v>85</v>
+        <v>122</v>
+      </c>
+    </row>
+    <row r="32" spans="2:6" ht="18" x14ac:dyDescent="0.35">
+      <c r="B32" s="4" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="33" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B33" t="s">
+        <v>47</v>
+      </c>
       <c r="C33" t="s">
-        <v>106</v>
+        <v>73</v>
       </c>
       <c r="D33" s="3">
-        <v>4</v>
-      </c>
-      <c r="E33" t="s">
-        <v>107</v>
+        <v>1</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="F33" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="34" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B34" t="s">
-        <v>97</v>
+        <v>74</v>
       </c>
       <c r="C34" t="s">
-        <v>98</v>
+        <v>76</v>
       </c>
       <c r="D34" s="3">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E34" t="s">
-        <v>99</v>
+        <v>33</v>
+      </c>
+      <c r="F34" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="35" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B35" t="s">
-        <v>21</v>
+        <v>75</v>
       </c>
       <c r="C35" t="s">
+        <v>77</v>
+      </c>
+      <c r="D35" s="3">
+        <v>1</v>
+      </c>
+      <c r="E35" t="s">
+        <v>79</v>
+      </c>
+      <c r="F35" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="36" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B36" t="s">
+        <v>87</v>
+      </c>
+      <c r="C36" t="s">
+        <v>84</v>
+      </c>
+      <c r="D36" s="3">
+        <v>4</v>
+      </c>
+      <c r="E36" t="s">
+        <v>85</v>
+      </c>
+      <c r="F36" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="37" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B37" t="s">
+        <v>63</v>
+      </c>
+      <c r="C37" t="s">
+        <v>80</v>
+      </c>
+      <c r="D37" s="3">
+        <v>1</v>
+      </c>
+      <c r="E37" t="s">
+        <v>82</v>
+      </c>
+      <c r="F37" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="38" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="C38" t="s">
+        <v>103</v>
+      </c>
+      <c r="D38" s="3">
+        <v>4</v>
+      </c>
+      <c r="E38" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="39" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B39" t="s">
+        <v>94</v>
+      </c>
+      <c r="C39" t="s">
         <v>95</v>
       </c>
-      <c r="D35" s="3">
-        <v>1</v>
-      </c>
-      <c r="E35" t="s">
-        <v>93</v>
-      </c>
-      <c r="F35" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="36" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="E36" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="37" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="E37" t="s">
+      <c r="D39" s="3">
+        <v>1</v>
+      </c>
+      <c r="E39" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="39" spans="2:6" ht="18" x14ac:dyDescent="0.35">
-      <c r="B39" s="4" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="41" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B41" t="s">
-        <v>101</v>
-      </c>
-      <c r="C41" t="s">
-        <v>39</v>
-      </c>
-      <c r="D41" s="3">
+    <row r="44" spans="2:6" ht="18" x14ac:dyDescent="0.35">
+      <c r="B44" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="46" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B46" t="s">
+        <v>98</v>
+      </c>
+      <c r="C46" t="s">
+        <v>37</v>
+      </c>
+      <c r="D46" s="3">
         <v>3</v>
       </c>
-      <c r="E41" t="s">
-        <v>32</v>
-      </c>
-      <c r="F41" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="42" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B42" t="s">
-        <v>5</v>
-      </c>
-      <c r="C42" t="s">
-        <v>78</v>
-      </c>
-      <c r="D42" s="3">
-        <v>3</v>
-      </c>
-      <c r="E42" t="s">
-        <v>35</v>
-      </c>
-      <c r="F42" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="43" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B43" t="s">
-        <v>102</v>
-      </c>
-      <c r="C43" t="s">
-        <v>10</v>
-      </c>
-      <c r="D43" s="3">
-        <v>1</v>
-      </c>
-      <c r="E43" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F43" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="44" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B44" t="s">
-        <v>89</v>
-      </c>
-      <c r="C44" t="s">
-        <v>86</v>
-      </c>
-      <c r="D44" s="3">
-        <v>4</v>
-      </c>
-      <c r="E44" t="s">
-        <v>91</v>
-      </c>
-      <c r="F44" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="45" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B45" t="s">
-        <v>103</v>
-      </c>
-      <c r="C45" t="s">
-        <v>45</v>
-      </c>
-      <c r="D45" s="3">
-        <v>1</v>
-      </c>
-      <c r="E45" t="s">
-        <v>46</v>
-      </c>
-      <c r="F45" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="46" spans="2:6" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B46" t="s">
-        <v>33</v>
-      </c>
-      <c r="C46" t="s">
-        <v>34</v>
-      </c>
-      <c r="D46" s="3">
-        <v>1</v>
-      </c>
-      <c r="E46" s="2" t="s">
-        <v>48</v>
+      <c r="E46" t="s">
+        <v>30</v>
       </c>
       <c r="F46" t="s">
-        <v>62</v>
+        <v>29</v>
       </c>
     </row>
     <row r="47" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B47" t="s">
-        <v>37</v>
+        <v>5</v>
       </c>
       <c r="C47" t="s">
-        <v>38</v>
+        <v>76</v>
       </c>
       <c r="D47" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E47" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="F47" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
     </row>
     <row r="48" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B48" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="C48" t="s">
-        <v>105</v>
+        <v>10</v>
       </c>
       <c r="D48" s="3">
-        <v>3</v>
-      </c>
-      <c r="E48" t="s">
-        <v>69</v>
+        <v>1</v>
+      </c>
+      <c r="E48" s="2" t="s">
+        <v>11</v>
       </c>
       <c r="F48" t="s">
-        <v>70</v>
+        <v>13</v>
       </c>
     </row>
     <row r="49" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B49" t="s">
-        <v>108</v>
+        <v>87</v>
       </c>
       <c r="C49" t="s">
-        <v>109</v>
+        <v>84</v>
       </c>
       <c r="D49" s="3">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E49" t="s">
-        <v>110</v>
+        <v>89</v>
       </c>
       <c r="F49" t="s">
-        <v>111</v>
+        <v>86</v>
       </c>
     </row>
     <row r="50" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B50" t="s">
+        <v>100</v>
+      </c>
+      <c r="C50" t="s">
+        <v>43</v>
+      </c>
+      <c r="D50" s="3">
+        <v>1</v>
+      </c>
+      <c r="E50" t="s">
+        <v>44</v>
+      </c>
+      <c r="F50" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="51" spans="2:6" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B51" t="s">
+        <v>31</v>
+      </c>
+      <c r="C51" t="s">
+        <v>32</v>
+      </c>
+      <c r="D51" s="3">
+        <v>1</v>
+      </c>
+      <c r="E51" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F51" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="52" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B52" t="s">
+        <v>35</v>
+      </c>
+      <c r="C52" t="s">
+        <v>36</v>
+      </c>
+      <c r="D52" s="3">
+        <v>1</v>
+      </c>
+      <c r="E52" t="s">
+        <v>39</v>
+      </c>
+      <c r="F52" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="53" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B53" t="s">
+        <v>101</v>
+      </c>
+      <c r="C53" t="s">
+        <v>102</v>
+      </c>
+      <c r="D53" s="3">
+        <v>3</v>
+      </c>
+      <c r="E53" t="s">
+        <v>67</v>
+      </c>
+      <c r="F53" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="54" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B54" t="s">
+        <v>105</v>
+      </c>
+      <c r="C54" t="s">
+        <v>106</v>
+      </c>
+      <c r="D54" s="3">
+        <v>1</v>
+      </c>
+      <c r="E54" t="s">
+        <v>107</v>
+      </c>
+      <c r="F54" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="55" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B55" t="s">
+        <v>109</v>
+      </c>
+      <c r="C55" t="s">
+        <v>84</v>
+      </c>
+      <c r="D55" s="3">
+        <v>4</v>
+      </c>
+      <c r="E55" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="56" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B56" t="s">
+        <v>111</v>
+      </c>
+      <c r="E56" t="s">
         <v>112</v>
       </c>
-      <c r="C50" t="s">
-        <v>86</v>
-      </c>
-      <c r="D50" s="3">
-        <v>4</v>
-      </c>
-      <c r="E50" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="51" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B51" t="s">
-        <v>114</v>
-      </c>
-      <c r="E51" t="s">
-        <v>115</v>
+    </row>
+    <row r="57" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B57" t="s">
+        <v>21</v>
+      </c>
+      <c r="C57" t="s">
+        <v>93</v>
+      </c>
+      <c r="D57" s="3">
+        <v>1</v>
+      </c>
+      <c r="E57" t="s">
+        <v>91</v>
+      </c>
+      <c r="F57" t="s">
+        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>